<commit_message>
Add BMI for 0~13w
</commit_message>
<xml_diff>
--- a/excel/all_0_13.xlsx
+++ b/excel/all_0_13.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repos\child_growth_chart\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9416E165-ED78-4668-88E7-0939F8AF59D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09BC08D4-12E5-4103-9A08-621F7F79292E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2850" yWindow="2850" windowWidth="21600" windowHeight="11332" activeTab="2" xr2:uid="{A7E86D5E-0232-4A53-A26D-0E9CC10B374C}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10276" activeTab="3" xr2:uid="{A7E86D5E-0232-4A53-A26D-0E9CC10B374C}"/>
   </bookViews>
   <sheets>
     <sheet name="Length" sheetId="2" r:id="rId1"/>
     <sheet name="Weight" sheetId="3" r:id="rId2"/>
     <sheet name="Head Circumference" sheetId="4" r:id="rId3"/>
+    <sheet name="BMI" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="21">
   <si>
     <t>Y</t>
   </si>
@@ -156,9 +157,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -196,7 +197,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -302,7 +303,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -444,7 +445,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2305,7 +2306,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CC7E9DA-E8ED-45D0-9CFC-D1E8B3900457}">
   <dimension ref="A1:U15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="N20" sqref="N20"/>
     </sheetView>
   </sheetViews>
@@ -3242,6 +3243,909 @@
       </c>
       <c r="T15">
         <v>44.2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83E3AD6F-2E88-4A0B-BBCF-FBD5D16EDA53}">
+  <dimension ref="A1:T15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" t="s">
+        <v>8</v>
+      </c>
+      <c r="M1" t="s">
+        <v>7</v>
+      </c>
+      <c r="N1" t="s">
+        <v>6</v>
+      </c>
+      <c r="O1" t="s">
+        <v>5</v>
+      </c>
+      <c r="P1" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>3</v>
+      </c>
+      <c r="R1" t="s">
+        <v>2</v>
+      </c>
+      <c r="S1" t="s">
+        <v>1</v>
+      </c>
+      <c r="T1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>-0.30530000000000002</v>
+      </c>
+      <c r="C2">
+        <v>13.4069</v>
+      </c>
+      <c r="D2">
+        <v>9.5600000000000004E-2</v>
+      </c>
+      <c r="E2">
+        <v>10.1</v>
+      </c>
+      <c r="F2">
+        <v>10.8</v>
+      </c>
+      <c r="G2">
+        <v>11.3</v>
+      </c>
+      <c r="H2">
+        <v>11.5</v>
+      </c>
+      <c r="I2">
+        <v>11.9</v>
+      </c>
+      <c r="J2">
+        <v>12.2</v>
+      </c>
+      <c r="K2">
+        <v>12.6</v>
+      </c>
+      <c r="L2">
+        <v>13.4</v>
+      </c>
+      <c r="M2">
+        <v>14.3</v>
+      </c>
+      <c r="N2">
+        <v>14.8</v>
+      </c>
+      <c r="O2">
+        <v>15.2</v>
+      </c>
+      <c r="P2">
+        <v>15.8</v>
+      </c>
+      <c r="Q2">
+        <v>16.100000000000001</v>
+      </c>
+      <c r="R2">
+        <v>16.899999999999999</v>
+      </c>
+      <c r="S2">
+        <v>18.3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>0.52470000000000006</v>
+      </c>
+      <c r="C3">
+        <v>13.3421</v>
+      </c>
+      <c r="D3">
+        <v>9.8210000000000006E-2</v>
+      </c>
+      <c r="E3">
+        <v>9.6</v>
+      </c>
+      <c r="F3">
+        <v>10.5</v>
+      </c>
+      <c r="G3">
+        <v>11</v>
+      </c>
+      <c r="H3">
+        <v>11.3</v>
+      </c>
+      <c r="I3">
+        <v>11.7</v>
+      </c>
+      <c r="J3">
+        <v>12</v>
+      </c>
+      <c r="K3">
+        <v>12.5</v>
+      </c>
+      <c r="L3">
+        <v>13.3</v>
+      </c>
+      <c r="M3">
+        <v>14.2</v>
+      </c>
+      <c r="N3">
+        <v>14.7</v>
+      </c>
+      <c r="O3">
+        <v>15.1</v>
+      </c>
+      <c r="P3">
+        <v>15.6</v>
+      </c>
+      <c r="Q3">
+        <v>15.9</v>
+      </c>
+      <c r="R3">
+        <v>16.600000000000001</v>
+      </c>
+      <c r="S3">
+        <v>17.7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>0.41770000000000002</v>
+      </c>
+      <c r="C4">
+        <v>13.637700000000001</v>
+      </c>
+      <c r="D4">
+        <v>9.4539999999999999E-2</v>
+      </c>
+      <c r="E4">
+        <v>10</v>
+      </c>
+      <c r="F4">
+        <v>10.8</v>
+      </c>
+      <c r="G4">
+        <v>11.3</v>
+      </c>
+      <c r="H4">
+        <v>11.6</v>
+      </c>
+      <c r="I4">
+        <v>12</v>
+      </c>
+      <c r="J4">
+        <v>12.3</v>
+      </c>
+      <c r="K4">
+        <v>12.8</v>
+      </c>
+      <c r="L4">
+        <v>13.6</v>
+      </c>
+      <c r="M4">
+        <v>14.5</v>
+      </c>
+      <c r="N4">
+        <v>15</v>
+      </c>
+      <c r="O4">
+        <v>15.3</v>
+      </c>
+      <c r="P4">
+        <v>15.9</v>
+      </c>
+      <c r="Q4">
+        <v>16.2</v>
+      </c>
+      <c r="R4">
+        <v>16.8</v>
+      </c>
+      <c r="S4">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>0.34489999999999998</v>
+      </c>
+      <c r="C5">
+        <v>14.2241</v>
+      </c>
+      <c r="D5">
+        <v>9.2299999999999993E-2</v>
+      </c>
+      <c r="E5">
+        <v>10.5</v>
+      </c>
+      <c r="F5">
+        <v>11.4</v>
+      </c>
+      <c r="G5">
+        <v>11.9</v>
+      </c>
+      <c r="H5">
+        <v>12.2</v>
+      </c>
+      <c r="I5">
+        <v>12.6</v>
+      </c>
+      <c r="J5">
+        <v>12.9</v>
+      </c>
+      <c r="K5">
+        <v>13.4</v>
+      </c>
+      <c r="L5">
+        <v>14.2</v>
+      </c>
+      <c r="M5">
+        <v>15.1</v>
+      </c>
+      <c r="N5">
+        <v>15.6</v>
+      </c>
+      <c r="O5">
+        <v>16</v>
+      </c>
+      <c r="P5">
+        <v>16.5</v>
+      </c>
+      <c r="Q5">
+        <v>16.8</v>
+      </c>
+      <c r="R5">
+        <v>17.5</v>
+      </c>
+      <c r="S5">
+        <v>18.7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>0.28810000000000002</v>
+      </c>
+      <c r="C6">
+        <v>14.7714</v>
+      </c>
+      <c r="D6">
+        <v>9.0719999999999995E-2</v>
+      </c>
+      <c r="E6">
+        <v>11</v>
+      </c>
+      <c r="F6">
+        <v>11.9</v>
+      </c>
+      <c r="G6">
+        <v>12.4</v>
+      </c>
+      <c r="H6">
+        <v>12.7</v>
+      </c>
+      <c r="I6">
+        <v>13.1</v>
+      </c>
+      <c r="J6">
+        <v>13.4</v>
+      </c>
+      <c r="K6">
+        <v>13.9</v>
+      </c>
+      <c r="L6">
+        <v>14.8</v>
+      </c>
+      <c r="M6">
+        <v>15.7</v>
+      </c>
+      <c r="N6">
+        <v>16.2</v>
+      </c>
+      <c r="O6">
+        <v>16.600000000000001</v>
+      </c>
+      <c r="P6">
+        <v>17.100000000000001</v>
+      </c>
+      <c r="Q6">
+        <v>17.399999999999999</v>
+      </c>
+      <c r="R6">
+        <v>18.100000000000001</v>
+      </c>
+      <c r="S6">
+        <v>19.3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>0.2409</v>
+      </c>
+      <c r="C7">
+        <v>15.2355</v>
+      </c>
+      <c r="D7">
+        <v>8.9529999999999998E-2</v>
+      </c>
+      <c r="E7">
+        <v>11.4</v>
+      </c>
+      <c r="F7">
+        <v>12.3</v>
+      </c>
+      <c r="G7">
+        <v>12.8</v>
+      </c>
+      <c r="H7">
+        <v>13.1</v>
+      </c>
+      <c r="I7">
+        <v>13.6</v>
+      </c>
+      <c r="J7">
+        <v>13.9</v>
+      </c>
+      <c r="K7">
+        <v>14.3</v>
+      </c>
+      <c r="L7">
+        <v>15.2</v>
+      </c>
+      <c r="M7">
+        <v>16.2</v>
+      </c>
+      <c r="N7">
+        <v>16.7</v>
+      </c>
+      <c r="O7">
+        <v>17.100000000000001</v>
+      </c>
+      <c r="P7">
+        <v>17.600000000000001</v>
+      </c>
+      <c r="Q7">
+        <v>18</v>
+      </c>
+      <c r="R7">
+        <v>18.7</v>
+      </c>
+      <c r="S7">
+        <v>19.899999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>0.20030000000000001</v>
+      </c>
+      <c r="C8">
+        <v>15.6107</v>
+      </c>
+      <c r="D8">
+        <v>8.8590000000000002E-2</v>
+      </c>
+      <c r="E8">
+        <v>11.8</v>
+      </c>
+      <c r="F8">
+        <v>12.6</v>
+      </c>
+      <c r="G8">
+        <v>13.2</v>
+      </c>
+      <c r="H8">
+        <v>13.5</v>
+      </c>
+      <c r="I8">
+        <v>13.9</v>
+      </c>
+      <c r="J8">
+        <v>14.2</v>
+      </c>
+      <c r="K8">
+        <v>14.7</v>
+      </c>
+      <c r="L8">
+        <v>15.6</v>
+      </c>
+      <c r="M8">
+        <v>16.600000000000001</v>
+      </c>
+      <c r="N8">
+        <v>17.100000000000001</v>
+      </c>
+      <c r="O8">
+        <v>17.5</v>
+      </c>
+      <c r="P8">
+        <v>18</v>
+      </c>
+      <c r="Q8">
+        <v>18.399999999999999</v>
+      </c>
+      <c r="R8">
+        <v>19.100000000000001</v>
+      </c>
+      <c r="S8">
+        <v>20.399999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>0.16450000000000001</v>
+      </c>
+      <c r="C9">
+        <v>15.9169</v>
+      </c>
+      <c r="D9">
+        <v>8.7819999999999995E-2</v>
+      </c>
+      <c r="E9">
+        <v>12.1</v>
+      </c>
+      <c r="F9">
+        <v>12.9</v>
+      </c>
+      <c r="G9">
+        <v>13.5</v>
+      </c>
+      <c r="H9">
+        <v>13.8</v>
+      </c>
+      <c r="I9">
+        <v>14.2</v>
+      </c>
+      <c r="J9">
+        <v>14.5</v>
+      </c>
+      <c r="K9">
+        <v>15</v>
+      </c>
+      <c r="L9">
+        <v>15.9</v>
+      </c>
+      <c r="M9">
+        <v>16.899999999999999</v>
+      </c>
+      <c r="N9">
+        <v>17.399999999999999</v>
+      </c>
+      <c r="O9">
+        <v>17.8</v>
+      </c>
+      <c r="P9">
+        <v>18.399999999999999</v>
+      </c>
+      <c r="Q9">
+        <v>18.7</v>
+      </c>
+      <c r="R9">
+        <v>19.5</v>
+      </c>
+      <c r="S9">
+        <v>20.8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>0.13239999999999999</v>
+      </c>
+      <c r="C10">
+        <v>16.169799999999999</v>
+      </c>
+      <c r="D10">
+        <v>8.7169999999999997E-2</v>
+      </c>
+      <c r="E10">
+        <v>12.3</v>
+      </c>
+      <c r="F10">
+        <v>13.2</v>
+      </c>
+      <c r="G10">
+        <v>13.7</v>
+      </c>
+      <c r="H10">
+        <v>14</v>
+      </c>
+      <c r="I10">
+        <v>14.4</v>
+      </c>
+      <c r="J10">
+        <v>14.8</v>
+      </c>
+      <c r="K10">
+        <v>15.2</v>
+      </c>
+      <c r="L10">
+        <v>16.2</v>
+      </c>
+      <c r="M10">
+        <v>17.100000000000001</v>
+      </c>
+      <c r="N10">
+        <v>17.7</v>
+      </c>
+      <c r="O10">
+        <v>18.100000000000001</v>
+      </c>
+      <c r="P10">
+        <v>18.600000000000001</v>
+      </c>
+      <c r="Q10">
+        <v>19</v>
+      </c>
+      <c r="R10">
+        <v>19.8</v>
+      </c>
+      <c r="S10">
+        <v>21.1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>0.1032</v>
+      </c>
+      <c r="C11">
+        <v>16.378699999999998</v>
+      </c>
+      <c r="D11">
+        <v>8.6610000000000006E-2</v>
+      </c>
+      <c r="E11">
+        <v>12.5</v>
+      </c>
+      <c r="F11">
+        <v>13.4</v>
+      </c>
+      <c r="G11">
+        <v>13.9</v>
+      </c>
+      <c r="H11">
+        <v>14.2</v>
+      </c>
+      <c r="I11">
+        <v>14.6</v>
+      </c>
+      <c r="J11">
+        <v>15</v>
+      </c>
+      <c r="K11">
+        <v>15.4</v>
+      </c>
+      <c r="L11">
+        <v>16.399999999999999</v>
+      </c>
+      <c r="M11">
+        <v>17.399999999999999</v>
+      </c>
+      <c r="N11">
+        <v>17.899999999999999</v>
+      </c>
+      <c r="O11">
+        <v>18.3</v>
+      </c>
+      <c r="P11">
+        <v>18.899999999999999</v>
+      </c>
+      <c r="Q11">
+        <v>19.3</v>
+      </c>
+      <c r="R11">
+        <v>20</v>
+      </c>
+      <c r="S11">
+        <v>21.3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>7.6600000000000001E-2</v>
+      </c>
+      <c r="C12">
+        <v>16.549399999999999</v>
+      </c>
+      <c r="D12">
+        <v>8.6120000000000002E-2</v>
+      </c>
+      <c r="E12">
+        <v>12.6</v>
+      </c>
+      <c r="F12">
+        <v>13.5</v>
+      </c>
+      <c r="G12">
+        <v>14.1</v>
+      </c>
+      <c r="H12">
+        <v>14.4</v>
+      </c>
+      <c r="I12">
+        <v>14.8</v>
+      </c>
+      <c r="J12">
+        <v>15.1</v>
+      </c>
+      <c r="K12">
+        <v>15.6</v>
+      </c>
+      <c r="L12">
+        <v>16.5</v>
+      </c>
+      <c r="M12">
+        <v>17.5</v>
+      </c>
+      <c r="N12">
+        <v>18.100000000000001</v>
+      </c>
+      <c r="O12">
+        <v>18.5</v>
+      </c>
+      <c r="P12">
+        <v>19.100000000000001</v>
+      </c>
+      <c r="Q12">
+        <v>19.399999999999999</v>
+      </c>
+      <c r="R12">
+        <v>20.2</v>
+      </c>
+      <c r="S12">
+        <v>21.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <v>5.1999999999999998E-2</v>
+      </c>
+      <c r="C13">
+        <v>16.688199999999998</v>
+      </c>
+      <c r="D13">
+        <v>8.5690000000000002E-2</v>
+      </c>
+      <c r="E13">
+        <v>12.8</v>
+      </c>
+      <c r="F13">
+        <v>13.7</v>
+      </c>
+      <c r="G13">
+        <v>14.2</v>
+      </c>
+      <c r="H13">
+        <v>14.5</v>
+      </c>
+      <c r="I13">
+        <v>14.9</v>
+      </c>
+      <c r="J13">
+        <v>15.3</v>
+      </c>
+      <c r="K13">
+        <v>15.7</v>
+      </c>
+      <c r="L13">
+        <v>16.7</v>
+      </c>
+      <c r="M13">
+        <v>17.7</v>
+      </c>
+      <c r="N13">
+        <v>18.2</v>
+      </c>
+      <c r="O13">
+        <v>18.600000000000001</v>
+      </c>
+      <c r="P13">
+        <v>19.2</v>
+      </c>
+      <c r="Q13">
+        <v>19.600000000000001</v>
+      </c>
+      <c r="R13">
+        <v>20.3</v>
+      </c>
+      <c r="S13">
+        <v>21.7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <v>2.9100000000000001E-2</v>
+      </c>
+      <c r="C14">
+        <v>16.801600000000001</v>
+      </c>
+      <c r="D14">
+        <v>8.5309999999999997E-2</v>
+      </c>
+      <c r="E14">
+        <v>12.9</v>
+      </c>
+      <c r="F14">
+        <v>13.8</v>
+      </c>
+      <c r="G14">
+        <v>14.3</v>
+      </c>
+      <c r="H14">
+        <v>14.6</v>
+      </c>
+      <c r="I14">
+        <v>15.1</v>
+      </c>
+      <c r="J14">
+        <v>15.4</v>
+      </c>
+      <c r="K14">
+        <v>15.9</v>
+      </c>
+      <c r="L14">
+        <v>16.8</v>
+      </c>
+      <c r="M14">
+        <v>17.8</v>
+      </c>
+      <c r="N14">
+        <v>18.399999999999999</v>
+      </c>
+      <c r="O14">
+        <v>18.7</v>
+      </c>
+      <c r="P14">
+        <v>19.3</v>
+      </c>
+      <c r="Q14">
+        <v>19.7</v>
+      </c>
+      <c r="R14">
+        <v>20.5</v>
+      </c>
+      <c r="S14">
+        <v>21.8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15">
+        <v>7.7000000000000002E-3</v>
+      </c>
+      <c r="C15">
+        <v>16.895</v>
+      </c>
+      <c r="D15">
+        <v>8.4959999999999994E-2</v>
+      </c>
+      <c r="E15">
+        <v>13</v>
+      </c>
+      <c r="F15">
+        <v>13.9</v>
+      </c>
+      <c r="G15">
+        <v>14.4</v>
+      </c>
+      <c r="H15">
+        <v>14.7</v>
+      </c>
+      <c r="I15">
+        <v>15.2</v>
+      </c>
+      <c r="J15">
+        <v>15.5</v>
+      </c>
+      <c r="K15">
+        <v>16</v>
+      </c>
+      <c r="L15">
+        <v>16.899999999999999</v>
+      </c>
+      <c r="M15">
+        <v>17.899999999999999</v>
+      </c>
+      <c r="N15">
+        <v>18.399999999999999</v>
+      </c>
+      <c r="O15">
+        <v>18.8</v>
+      </c>
+      <c r="P15">
+        <v>19.399999999999999</v>
+      </c>
+      <c r="Q15">
+        <v>19.8</v>
+      </c>
+      <c r="R15">
+        <v>20.6</v>
+      </c>
+      <c r="S15">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add 1m weight data
</commit_message>
<xml_diff>
--- a/excel/all_0_13.xlsx
+++ b/excel/all_0_13.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lingxl\Desktop\repos\child_growth_chart\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9337920E-B5BF-45CB-860F-FC6F7280B40A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{657BF3DB-6CE3-487A-8611-03303144A6B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5895" yWindow="3938" windowWidth="21600" windowHeight="11332" activeTab="2" xr2:uid="{A7E86D5E-0232-4A53-A26D-0E9CC10B374C}"/>
+    <workbookView xWindow="5895" yWindow="3938" windowWidth="21600" windowHeight="11332" activeTab="1" xr2:uid="{A7E86D5E-0232-4A53-A26D-0E9CC10B374C}"/>
   </bookViews>
   <sheets>
     <sheet name="Length" sheetId="2" r:id="rId1"/>
@@ -157,7 +157,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
     <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
@@ -445,7 +445,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1412,8 +1412,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7109A73-9D57-4BCA-B466-9D1281C44465}">
   <dimension ref="A1:T15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="R21" sqref="R21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T7" sqref="T7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1785,6 +1785,9 @@
       </c>
       <c r="S6">
         <v>6.5</v>
+      </c>
+      <c r="T6">
+        <v>5.66</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.45">
@@ -2327,7 +2330,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CC7E9DA-E8ED-45D0-9CFC-D1E8B3900457}">
   <dimension ref="A1:U15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="U5" sqref="U5"/>
     </sheetView>
   </sheetViews>

</xml_diff>